<commit_message>
understanding formula sheet added
</commit_message>
<xml_diff>
--- a/excel-beginner-tutorial.xlsx
+++ b/excel-beginner-tutorial.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects\microsoft-excel-tutorial-beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1541B47-130B-4494-90D7-9D185CC34961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3066F873-CE7F-4AA7-8130-B5383C5518D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="9" xr2:uid="{9FA7835E-DA76-4B93-946E-CCC2848369CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="5" activeTab="14" xr2:uid="{9FA7835E-DA76-4B93-946E-CCC2848369CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
     <sheet name="DataTypes" sheetId="14" r:id="rId2"/>
     <sheet name="Logical and Condi State." sheetId="15" r:id="rId3"/>
     <sheet name="Formatting" sheetId="2" r:id="rId4"/>
-    <sheet name="Text" sheetId="4" r:id="rId5"/>
-    <sheet name="Table" sheetId="3" r:id="rId6"/>
-    <sheet name="AbsoluteAndRelative" sheetId="9" r:id="rId7"/>
-    <sheet name="Vlookup simple" sheetId="11" r:id="rId8"/>
-    <sheet name="Vlookup 1" sheetId="10" r:id="rId9"/>
-    <sheet name="Vlookup 2" sheetId="8" r:id="rId10"/>
-    <sheet name="Vlookup Scenario" sheetId="13" r:id="rId11"/>
-    <sheet name="Shortcut Keys" sheetId="12" r:id="rId12"/>
-    <sheet name="Pivot" sheetId="5" r:id="rId13"/>
-    <sheet name="Pivot (2)" sheetId="7" r:id="rId14"/>
+    <sheet name="Understanding Formula" sheetId="16" r:id="rId5"/>
+    <sheet name="Text" sheetId="4" r:id="rId6"/>
+    <sheet name="Table" sheetId="3" r:id="rId7"/>
+    <sheet name="AbsoluteAndRelative" sheetId="9" r:id="rId8"/>
+    <sheet name="Vlookup simple" sheetId="11" r:id="rId9"/>
+    <sheet name="Vlookup 1" sheetId="10" r:id="rId10"/>
+    <sheet name="Vlookup 2" sheetId="8" r:id="rId11"/>
+    <sheet name="Vlookup Scenario" sheetId="13" r:id="rId12"/>
+    <sheet name="Shortcut Keys" sheetId="12" r:id="rId13"/>
+    <sheet name="Pivot" sheetId="5" r:id="rId14"/>
+    <sheet name="Pivot (2)" sheetId="7" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Text!$A$1:$B$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Text!$A$1:$B$51</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="713">
   <si>
     <t>Reg No.</t>
   </si>
@@ -2174,6 +2175,45 @@
   </si>
   <si>
     <t>Full Name</t>
+  </si>
+  <si>
+    <t>=F2=F3</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Sample Data</t>
+  </si>
+  <si>
+    <t>=G2&lt;&gt;G3</t>
+  </si>
+  <si>
+    <t>=H2&gt;H3</t>
+  </si>
+  <si>
+    <t>=I2&lt;I3</t>
+  </si>
+  <si>
+    <t>=I2&lt;=I3</t>
+  </si>
+  <si>
+    <t>=H2&gt;=H3</t>
+  </si>
+  <si>
+    <t>=AND(D3:D5)</t>
+  </si>
+  <si>
+    <t>=OR(D3:D8)</t>
+  </si>
+  <si>
+    <t>=NOT(D8)</t>
+  </si>
+  <si>
+    <t>https://exceljet.net/formulas</t>
+  </si>
+  <si>
+    <t>=IF(logical_test,value_if_true,value_if_false)</t>
   </si>
 </sst>
 </file>
@@ -2378,7 +2418,6 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2399,44 +2438,16 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{C317EB46-FD19-411F-B09C-9673D28024EA}"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -2462,50 +2473,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -3237,6 +3204,444 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Intro To Formula">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322208D4-F4B9-ADDD-ABCD-E404A4586E98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133349" y="109537"/>
+          <a:ext cx="5343526" cy="1281114"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>Understanding</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1" baseline="0"/>
+            <a:t> Formula and Its Syntax:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
+            <a:t>	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Formulas in Excel start with an equal sign (=) and can be composed of various functions, mathematical operators, and cell references.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> There are lot of formulas in excel for different purposes. Here we will be looking in to the most commonly used. Before hand its good to understand its syntax, so that it will be helpful to understand and explore other formulas as per your requirements.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>237945</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>139211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>197828</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43961</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Graphical user interface, application&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF9B34AE-511A-DFDC-364A-5F8E8D3C3956}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="61725" t="66343" r="20606" b="24723"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1454214" y="2615711"/>
+          <a:ext cx="3000556" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>70183</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>36345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>165434</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>115302</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Intro To Formula">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A61CEE8D-468C-6AC1-1F22-A985F5C8233E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="70183" y="1560345"/>
+          <a:ext cx="3153277" cy="269457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>Have</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t> a closer look at the below syntax of IF formula</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100" b="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>77202</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>148640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>140368</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>37097</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Intro To Formula">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0753611F-E7D1-1782-5AE6-C8B3A89E6804}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="77202" y="2244140"/>
+          <a:ext cx="3732798" cy="269457"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>You can find these</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t> syntax while typing any formula like below</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100" b="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>105044</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1384789</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>117230</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Intro To Formula">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A55FA596-2FDE-6B50-3064-03785DE0CE2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="105044" y="3546867"/>
+          <a:ext cx="5536687" cy="1332863"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>In</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t> case of IF formula you can pass up to 3 arguments separate by comma and if you closly look at the last two arguments are enclosed in square brackets unlike the 1st arguments. This is because these two arguments are optional arguments i.e. This formula works even if you do not pass the last two arguments.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100" b="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </a:rPr>
+            <a:t>Similarlly, have a look at a formula you have used before and try to understand its syntax.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100" b="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100" b="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{503F3CCD-0AAD-446E-97BA-E431AE00EECA}" name="Table2" displayName="Table2" ref="A1:G51" totalsRowShown="0">
   <autoFilter ref="A1:G51" xr:uid="{503F3CCD-0AAD-446E-97BA-E431AE00EECA}"/>
@@ -3556,50 +3961,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11" style="16" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="16" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="37.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11" style="15" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="40.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
+      <c r="A3" s="17"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="17"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="17"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+      <c r="A8" s="17"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="17"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="17"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="17"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
+      <c r="A12" s="17"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
+      <c r="A13" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3609,10 +4014,360 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C35B6DA-4005-4159-8F42-B0AFAD2CF07B}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C2" t="s">
+        <v>664</v>
+      </c>
+      <c r="D2" s="23">
+        <v>42535</v>
+      </c>
+      <c r="E2">
+        <v>12495185438</v>
+      </c>
+      <c r="F2" t="s">
+        <v>665</v>
+      </c>
+      <c r="G2" t="s">
+        <v>666</v>
+      </c>
+      <c r="H2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>668</v>
+      </c>
+      <c r="C3" t="s">
+        <v>669</v>
+      </c>
+      <c r="D3" s="23">
+        <v>42748</v>
+      </c>
+      <c r="E3">
+        <v>8109237463</v>
+      </c>
+      <c r="F3" t="s">
+        <v>665</v>
+      </c>
+      <c r="G3" t="s">
+        <v>670</v>
+      </c>
+      <c r="H3" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>672</v>
+      </c>
+      <c r="C4" t="s">
+        <v>673</v>
+      </c>
+      <c r="D4" s="23">
+        <v>42651</v>
+      </c>
+      <c r="E4">
+        <v>6653263786</v>
+      </c>
+      <c r="F4" t="s">
+        <v>665</v>
+      </c>
+      <c r="G4" t="s">
+        <v>666</v>
+      </c>
+      <c r="H4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>675</v>
+      </c>
+      <c r="C5" t="s">
+        <v>676</v>
+      </c>
+      <c r="D5" s="23">
+        <v>43222</v>
+      </c>
+      <c r="E5">
+        <v>6071073952</v>
+      </c>
+      <c r="F5" t="s">
+        <v>665</v>
+      </c>
+      <c r="G5" t="s">
+        <v>666</v>
+      </c>
+      <c r="H5" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>678</v>
+      </c>
+      <c r="C6" t="s">
+        <v>679</v>
+      </c>
+      <c r="D6" s="23">
+        <v>42765</v>
+      </c>
+      <c r="E6">
+        <v>5944830525</v>
+      </c>
+      <c r="F6" t="s">
+        <v>680</v>
+      </c>
+      <c r="G6" t="s">
+        <v>666</v>
+      </c>
+      <c r="H6" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>682</v>
+      </c>
+      <c r="C7" t="s">
+        <v>683</v>
+      </c>
+      <c r="D7" s="23">
+        <v>42101</v>
+      </c>
+      <c r="E7">
+        <v>5816307940</v>
+      </c>
+      <c r="F7" t="s">
+        <v>665</v>
+      </c>
+      <c r="G7" t="s">
+        <v>666</v>
+      </c>
+      <c r="H7" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>685</v>
+      </c>
+      <c r="C8" t="s">
+        <v>686</v>
+      </c>
+      <c r="D8" s="23">
+        <v>41704</v>
+      </c>
+      <c r="E8">
+        <v>5209038987</v>
+      </c>
+      <c r="F8" t="s">
+        <v>687</v>
+      </c>
+      <c r="G8" t="s">
+        <v>666</v>
+      </c>
+      <c r="H8" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>689</v>
+      </c>
+      <c r="C9" t="s">
+        <v>676</v>
+      </c>
+      <c r="D9" s="23">
+        <v>43244</v>
+      </c>
+      <c r="E9">
+        <v>5021165699</v>
+      </c>
+      <c r="F9" t="s">
+        <v>665</v>
+      </c>
+      <c r="G9" t="s">
+        <v>666</v>
+      </c>
+      <c r="H9" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>691</v>
+      </c>
+      <c r="C10" t="s">
+        <v>692</v>
+      </c>
+      <c r="D10" s="23">
+        <v>41962</v>
+      </c>
+      <c r="E10">
+        <v>4859631966</v>
+      </c>
+      <c r="F10" t="s">
+        <v>665</v>
+      </c>
+      <c r="G10" t="s">
+        <v>666</v>
+      </c>
+      <c r="H10" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>655</v>
+      </c>
+      <c r="H17" t="s">
+        <v>657</v>
+      </c>
+      <c r="I17" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="str">
+        <f>VLOOKUP($G18,$A$1:$H$10,3,FALSE)</f>
+        <v>LuisFonsiVEVO</v>
+      </c>
+      <c r="I18">
+        <f>VLOOKUP($G18,$A$1:$H$10,5,FALSE)</f>
+        <v>8109237463</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" ref="H19:H21" si="0">VLOOKUP($G19,$A$1:$H$10,3,FALSE)</f>
+        <v>Ed Sheeran</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I21" si="1">VLOOKUP($G19,$A$1:$H$10,5,FALSE)</f>
+        <v>5944830525</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>6</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>Wiz Khalifa</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>5816307940</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>MarkRonsonVEVO</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>4859631966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3C7C63A-B289-43DD-9A7C-2D11E4BAFA22}">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3633,20 +4388,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
       <c r="G1" t="s">
         <v>448</v>
       </c>
@@ -3694,8 +4449,8 @@
       <c r="D2" s="1">
         <v>501</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
       <c r="G2">
         <v>1</v>
       </c>
@@ -3726,7 +4481,7 @@
       <c r="V2" t="s">
         <v>435</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="12" t="s">
         <v>452</v>
       </c>
     </row>
@@ -3743,8 +4498,8 @@
       <c r="D3" s="1">
         <v>480</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
       <c r="G3">
         <v>7</v>
       </c>
@@ -3775,7 +4530,7 @@
       <c r="V3" t="s">
         <v>436</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="W3" s="12" t="s">
         <v>459</v>
       </c>
     </row>
@@ -3792,7 +4547,7 @@
       <c r="D4" s="1">
         <v>798</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="13"/>
       <c r="G4">
         <v>5</v>
       </c>
@@ -3823,7 +4578,7 @@
       <c r="V4" t="s">
         <v>437</v>
       </c>
-      <c r="W4" s="13" t="s">
+      <c r="W4" s="12" t="s">
         <v>465</v>
       </c>
     </row>
@@ -3840,8 +4595,8 @@
       <c r="D5" s="1">
         <v>798</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="L5">
         <v>25615256</v>
       </c>
@@ -3860,7 +4615,7 @@
       <c r="V5" t="s">
         <v>438</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="W5" s="12" t="s">
         <v>468</v>
       </c>
     </row>
@@ -3877,8 +4632,8 @@
       <c r="D6" s="1">
         <v>708</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
       <c r="L6">
         <v>25615257</v>
       </c>
@@ -3897,7 +4652,7 @@
       <c r="V6" t="s">
         <v>439</v>
       </c>
-      <c r="W6" s="13" t="s">
+      <c r="W6" s="12" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3914,8 +4669,8 @@
       <c r="D7" s="1">
         <v>501</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
       <c r="L7">
         <v>25615258</v>
       </c>
@@ -3925,7 +4680,7 @@
       <c r="V7" t="s">
         <v>440</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="12" t="s">
         <v>472</v>
       </c>
     </row>
@@ -3942,8 +4697,8 @@
       <c r="D8" s="1">
         <v>480</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="L8">
         <v>25615259</v>
       </c>
@@ -3953,7 +4708,7 @@
       <c r="V8" t="s">
         <v>441</v>
       </c>
-      <c r="W8" s="13" t="s">
+      <c r="W8" s="12" t="s">
         <v>457</v>
       </c>
     </row>
@@ -3970,8 +4725,8 @@
       <c r="D9" s="1">
         <v>501</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="L9">
         <v>25615260</v>
       </c>
@@ -3989,8 +4744,8 @@
       <c r="D10" s="1">
         <v>708</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="L10">
         <v>25615261</v>
       </c>
@@ -4008,8 +4763,8 @@
       <c r="D11" s="1">
         <v>798</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="L11">
         <v>25615262</v>
       </c>
@@ -4259,7 +5014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97242C3-98C7-4CC8-9E05-11ED756AE458}">
   <dimension ref="A1:I15"/>
   <sheetViews>
@@ -4388,7 +5143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108E1899-0BA1-4EAD-977B-5AF4891D964A}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -4607,7 +5362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B59B5EA-5F36-4506-9B80-2736CCDF45D1}">
   <dimension ref="A1:C201"/>
   <sheetViews>
@@ -6840,11 +7595,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB8F69F-168D-4701-80B4-C17E080F19B6}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -7982,92 +8737,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="20"/>
-    <col min="3" max="3" width="16.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="10" style="20" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="20"/>
-    <col min="7" max="7" width="12.7109375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="20"/>
-    <col min="9" max="9" width="15" style="20" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="2" width="9.140625" style="19"/>
+    <col min="3" max="3" width="20" style="19" customWidth="1"/>
+    <col min="4" max="4" width="10" style="19" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
+    <col min="7" max="7" width="13.7109375" style="19" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="19"/>
+    <col min="9" max="9" width="16.7109375" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>652</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="26"/>
+      <c r="E5" s="27" t="s">
         <v>650</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="25" t="s">
         <v>651</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="26" t="s">
+      <c r="H5" s="26"/>
+      <c r="I5" s="25" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>649</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27">
+      <c r="D6" s="26"/>
+      <c r="E6" s="26">
         <v>123</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27" t="b">
+      <c r="F6" s="26"/>
+      <c r="G6" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27" t="e" cm="1">
+      <c r="H6" s="26"/>
+      <c r="I6" s="26" t="e" cm="1">
         <f t="array" ref="I6">num</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26">
         <v>3.14</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27" t="b">
+      <c r="F7" s="26"/>
+      <c r="G7" s="26" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27" t="e">
+      <c r="H7" s="26"/>
+      <c r="I7" s="26" t="e">
         <f>SUM("TY")</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="29">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="28">
         <v>44956</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27" t="e">
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="30">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="29">
         <v>44974.951585648145</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27" t="e" cm="1">
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26" t="e" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">INDIRECT("")</f>
         <v>#REF!</v>
       </c>
@@ -8084,18 +8839,24 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="D1" s="30"/>
       <c r="F1" s="2" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -8105,6 +8866,12 @@
       <c r="B2" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="F2">
         <v>21</v>
       </c>
@@ -8112,7 +8879,7 @@
         <v>31</v>
       </c>
       <c r="H2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I2">
         <v>33</v>
@@ -8125,6 +8892,13 @@
       <c r="B3" t="s">
         <v>127</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="D3" t="b">
+        <f>F2=F3</f>
+        <v>1</v>
+      </c>
       <c r="F3">
         <v>21</v>
       </c>
@@ -8145,21 +8919,12 @@
       <c r="B4" t="s">
         <v>138</v>
       </c>
-      <c r="F4" t="b">
-        <f>F2=F3</f>
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
+      <c r="C4" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="D4" t="b">
         <f>G2&lt;&gt;G3</f>
         <v>1</v>
-      </c>
-      <c r="H4" t="b">
-        <f>H2&gt;H3</f>
-        <v>0</v>
-      </c>
-      <c r="I4" t="b">
-        <f>I2&lt;I3</f>
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -8169,6 +8934,13 @@
       <c r="B5" t="s">
         <v>145</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="D5" t="b">
+        <f>H2&gt;H3</f>
+        <v>1</v>
+      </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8178,17 +8950,12 @@
       <c r="B6" t="s">
         <v>152</v>
       </c>
-      <c r="F6" t="b">
-        <f>AND(F4,G4)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <f>OR(G4,H4)</f>
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <f>NOT(H4)</f>
-        <v>1</v>
+      <c r="C6" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="D6" t="b">
+        <f>I2&lt;I3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -8198,6 +8965,13 @@
       <c r="B7" t="s">
         <v>161</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="D7" t="b">
+        <f>H2&gt;=H3</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -8206,10 +8980,20 @@
       <c r="B8" t="s">
         <v>167</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="D8" t="b">
+        <f>I2&lt;=I3</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>181</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -8219,6 +9003,13 @@
       <c r="B12" t="s">
         <v>188</v>
       </c>
+      <c r="C12" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="D12" t="b">
+        <f>AND(D3:D5)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -8227,6 +9018,13 @@
       <c r="B13" t="s">
         <v>195</v>
       </c>
+      <c r="C13" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="D13" t="b">
+        <f>OR(D3:D8)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -8235,8 +9033,18 @@
       <c r="B14" t="s">
         <v>201</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="D14" t="b">
+        <f>NOT(D8)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8250,7 +9058,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8264,40 +9072,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>654</v>
       </c>
-      <c r="O1" s="22">
+      <c r="O1" s="21">
         <v>40</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -8305,36 +9113,36 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>77</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>65</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="21">
         <v>95</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="21">
         <v>84</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="21">
         <v>70</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <f>SUM(C2:G2)</f>
         <v>391</v>
       </c>
-      <c r="I2" s="22">
+      <c r="I2" s="21">
         <f>AVERAGE(C2:G2)</f>
         <v>78.2</v>
       </c>
-      <c r="J2" s="22" t="str">
+      <c r="J2" s="21" t="str">
         <f>IF(AND(C2&gt;=$O$1,D2&gt;=$O$1,E2&gt;=$O$1,F2&gt;=$O$1,G2&gt;=$O$1),"Pass","Fail")</f>
         <v>Pass</v>
       </c>
@@ -8343,36 +9151,36 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>88</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>90</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>86</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="21">
         <v>94</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="21">
         <v>73</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="21">
         <f t="shared" ref="H3:H51" si="0">SUM(C3:G3)</f>
         <v>431</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="21">
         <f t="shared" ref="I3:I51" si="1">AVERAGE(C3:G3)</f>
         <v>86.2</v>
       </c>
-      <c r="J3" s="22" t="str">
+      <c r="J3" s="21" t="str">
         <f t="shared" ref="J3:J51" si="2">IF(AND(C3&gt;=$O$1,D3&gt;=$O$1,E3&gt;=$O$1,F3&gt;=$O$1,G3&gt;=$O$1),"Pass","Fail")</f>
         <v>Pass</v>
       </c>
@@ -8381,36 +9189,36 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>84</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>69</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <v>69</v>
       </c>
-      <c r="F4" s="22">
-        <v>53</v>
-      </c>
-      <c r="G4" s="22">
+      <c r="F4" s="21">
+        <v>60</v>
+      </c>
+      <c r="G4" s="21">
         <v>72</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <f t="shared" si="0"/>
-        <v>347</v>
-      </c>
-      <c r="I4" s="22">
+        <v>354</v>
+      </c>
+      <c r="I4" s="21">
         <f t="shared" si="1"/>
-        <v>69.400000000000006</v>
-      </c>
-      <c r="J4" s="22" t="str">
+        <v>70.8</v>
+      </c>
+      <c r="J4" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8426,36 +9234,36 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>40</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>45</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>83</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>75</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>77</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="21">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="J5" s="22" t="str">
+      <c r="J5" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8471,36 +9279,36 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>47</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>70</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="21">
         <v>48</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>52</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>53</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <f t="shared" si="0"/>
         <v>270</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="21">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="J6" s="22" t="str">
+      <c r="J6" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8513,36 +9321,36 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>95</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>82</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>40</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>81</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="21">
         <v>92</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="21">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="J7" s="22" t="str">
+      <c r="J7" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8555,36 +9363,36 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>78</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <v>95</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>60</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="21">
         <v>85</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>89</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <f t="shared" si="0"/>
         <v>407</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="21">
         <f t="shared" si="1"/>
         <v>81.400000000000006</v>
       </c>
-      <c r="J8" s="22" t="str">
+      <c r="J8" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8597,71 +9405,71 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>97</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>48</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <v>76</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="21">
         <v>98</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="21">
         <v>86</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
         <f t="shared" si="0"/>
         <v>405</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="21">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="J9" s="22" t="str">
+      <c r="J9" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="21">
         <v>62</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>45</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <v>91</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="21">
         <v>88</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="21">
         <v>92</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <f t="shared" si="0"/>
         <v>378</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <f t="shared" si="1"/>
         <v>75.599999999999994</v>
       </c>
-      <c r="J10" s="22" t="str">
+      <c r="J10" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8675,176 +9483,176 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>45</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <v>59</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <v>69</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="21">
         <v>47</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="21">
         <v>68</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="21">
         <f t="shared" si="0"/>
         <v>288</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="21">
         <f t="shared" si="1"/>
         <v>57.6</v>
       </c>
-      <c r="J11" s="22" t="str">
+      <c r="J11" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="21">
         <v>51</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>45</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <v>84</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>93</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="21">
         <v>79</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
         <f t="shared" si="0"/>
         <v>352</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="21">
         <f t="shared" si="1"/>
         <v>70.400000000000006</v>
       </c>
-      <c r="J12" s="22" t="str">
+      <c r="J12" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="21">
         <v>84</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>60</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="21">
         <v>44</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>20</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="21">
         <v>41</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="21">
         <f t="shared" si="0"/>
         <v>249</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="21">
         <f t="shared" si="1"/>
         <v>49.8</v>
       </c>
-      <c r="J13" s="22" t="str">
+      <c r="J13" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="21">
         <v>90</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>63</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="21">
         <v>66</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>47</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="21">
         <v>97</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="21">
         <f t="shared" si="0"/>
         <v>363</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="21">
         <f t="shared" si="1"/>
         <v>72.599999999999994</v>
       </c>
-      <c r="J14" s="22" t="str">
+      <c r="J14" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="21">
         <v>86</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>63</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="21">
         <v>56</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>45</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="21">
         <v>78</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="21">
         <f t="shared" si="0"/>
         <v>328</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="21">
         <f t="shared" si="1"/>
         <v>65.599999999999994</v>
       </c>
-      <c r="J15" s="22" t="str">
+      <c r="J15" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8862,36 +9670,36 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="21">
         <v>75</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>81</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>70</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="21">
         <v>72</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="21">
         <v>61</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <f t="shared" si="0"/>
         <v>359</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="21">
         <f t="shared" si="1"/>
         <v>71.8</v>
       </c>
-      <c r="J16" s="22" t="str">
+      <c r="J16" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8911,36 +9719,36 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="21">
         <v>40</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>76</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>98</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="21">
         <v>66</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="21">
         <v>51</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <f t="shared" si="0"/>
         <v>331</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="21">
         <f t="shared" si="1"/>
         <v>66.2</v>
       </c>
-      <c r="J17" s="22" t="str">
+      <c r="J17" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -8960,36 +9768,36 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>53</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>65</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <v>79</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="21">
         <v>53</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="21">
         <v>39</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="21">
         <f t="shared" si="0"/>
         <v>289</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="21">
         <f t="shared" si="1"/>
         <v>57.8</v>
       </c>
-      <c r="J18" s="22" t="str">
+      <c r="J18" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
@@ -9009,36 +9817,36 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="21">
         <v>85</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>88</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="21">
         <v>100</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="21">
         <v>92</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="21">
         <v>98</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="21">
         <f t="shared" si="0"/>
         <v>463</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="21">
         <f t="shared" si="1"/>
         <v>92.6</v>
       </c>
-      <c r="J19" s="22" t="str">
+      <c r="J19" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
@@ -9058,1135 +9866,1135 @@
       </c>
     </row>
     <row r="20" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <v>89</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>91</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="21">
         <v>89</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <v>84</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="21">
         <v>77</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
         <f t="shared" si="0"/>
         <v>430</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="21">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="J20" s="22" t="str">
+      <c r="J20" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="21">
         <v>78</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="21">
         <v>78</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="21">
         <v>85</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="21">
         <v>47</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="21">
         <v>46</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="21">
         <f t="shared" si="0"/>
         <v>334</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="21">
         <f t="shared" si="1"/>
         <v>66.8</v>
       </c>
-      <c r="J21" s="22" t="str">
+      <c r="J21" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="21">
         <v>20</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="21">
         <v>57</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <v>88</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="21">
         <v>70</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="21">
         <v>41</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="21">
         <f t="shared" si="0"/>
         <v>276</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="21">
         <f t="shared" si="1"/>
         <v>55.2</v>
       </c>
-      <c r="J22" s="22" t="str">
+      <c r="J22" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="21">
         <v>65</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="21">
         <v>55</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <v>53</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="21">
         <v>75</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="21">
         <v>94</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="21">
         <f t="shared" si="0"/>
         <v>342</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="21">
         <f t="shared" si="1"/>
         <v>68.400000000000006</v>
       </c>
-      <c r="J23" s="22" t="str">
+      <c r="J23" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="21">
         <v>53</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="21">
         <v>92</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="21">
         <v>91</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="21">
         <v>48</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="21">
         <v>50</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="21">
         <f t="shared" si="0"/>
         <v>334</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="21">
         <f t="shared" si="1"/>
         <v>66.8</v>
       </c>
-      <c r="J24" s="22" t="str">
+      <c r="J24" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="21">
         <v>68</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="21">
         <v>53</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="21">
         <v>38</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="21">
         <v>85</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="21">
         <v>78</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="21">
         <f t="shared" si="0"/>
         <v>322</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="21">
         <f t="shared" si="1"/>
         <v>64.400000000000006</v>
       </c>
-      <c r="J25" s="22" t="str">
+      <c r="J25" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="21">
         <v>82</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <v>99</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="21">
         <v>88</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="21">
         <v>98</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="21">
         <v>95</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="21">
         <f t="shared" si="0"/>
         <v>462</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="21">
         <f t="shared" si="1"/>
         <v>92.4</v>
       </c>
-      <c r="J26" s="22" t="str">
+      <c r="J26" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="21">
         <v>73</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="21">
         <v>50</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="21">
         <v>73</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="21">
         <v>43</v>
       </c>
-      <c r="G27" s="22">
+      <c r="G27" s="21">
         <v>99</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="21">
         <f t="shared" si="0"/>
         <v>338</v>
       </c>
-      <c r="I27" s="22">
+      <c r="I27" s="21">
         <f t="shared" si="1"/>
         <v>67.599999999999994</v>
       </c>
-      <c r="J27" s="22" t="str">
+      <c r="J27" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="21">
         <v>93</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="21">
         <v>95</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="21">
         <v>49</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="21">
         <v>47</v>
       </c>
-      <c r="G28" s="22">
+      <c r="G28" s="21">
         <v>55</v>
       </c>
-      <c r="H28" s="22">
+      <c r="H28" s="21">
         <f t="shared" si="0"/>
         <v>339</v>
       </c>
-      <c r="I28" s="22">
+      <c r="I28" s="21">
         <f t="shared" si="1"/>
         <v>67.8</v>
       </c>
-      <c r="J28" s="22" t="str">
+      <c r="J28" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="21">
         <v>84</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="21">
         <v>92</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="21">
         <v>93</v>
       </c>
-      <c r="F29" s="22">
+      <c r="F29" s="21">
         <v>95</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="21">
         <v>80</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="21">
         <f t="shared" si="0"/>
         <v>444</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I29" s="21">
         <f t="shared" si="1"/>
         <v>88.8</v>
       </c>
-      <c r="J29" s="22" t="str">
+      <c r="J29" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30" s="21">
         <v>75</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="21">
         <v>91</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="21">
         <v>68</v>
       </c>
-      <c r="F30" s="22">
+      <c r="F30" s="21">
         <v>75</v>
       </c>
-      <c r="G30" s="22">
+      <c r="G30" s="21">
         <v>71</v>
       </c>
-      <c r="H30" s="22">
+      <c r="H30" s="21">
         <f t="shared" si="0"/>
         <v>380</v>
       </c>
-      <c r="I30" s="22">
+      <c r="I30" s="21">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="J30" s="22" t="str">
+      <c r="J30" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="21">
         <v>82</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="21">
         <v>89</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31" s="21">
         <v>57</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F31" s="21">
         <v>43</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G31" s="21">
         <v>47</v>
       </c>
-      <c r="H31" s="22">
+      <c r="H31" s="21">
         <f t="shared" si="0"/>
         <v>318</v>
       </c>
-      <c r="I31" s="22">
+      <c r="I31" s="21">
         <f t="shared" si="1"/>
         <v>63.6</v>
       </c>
-      <c r="J31" s="22" t="str">
+      <c r="J31" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="21">
         <v>72</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="21">
         <v>99</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32" s="21">
         <v>78</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="21">
         <v>92</v>
       </c>
-      <c r="G32" s="22">
+      <c r="G32" s="21">
         <v>78</v>
       </c>
-      <c r="H32" s="22">
+      <c r="H32" s="21">
         <f t="shared" si="0"/>
         <v>419</v>
       </c>
-      <c r="I32" s="22">
+      <c r="I32" s="21">
         <f t="shared" si="1"/>
         <v>83.8</v>
       </c>
-      <c r="J32" s="22" t="str">
+      <c r="J32" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="21">
         <v>89</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="21">
         <v>93</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="21">
         <v>68</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="21">
         <v>93</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="21">
         <v>83</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="21">
         <f t="shared" si="0"/>
         <v>426</v>
       </c>
-      <c r="I33" s="22">
+      <c r="I33" s="21">
         <f t="shared" si="1"/>
         <v>85.2</v>
       </c>
-      <c r="J33" s="22" t="str">
+      <c r="J33" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="21">
         <v>69</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="21">
         <v>67</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="21">
         <v>99</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="21">
         <v>74</v>
       </c>
-      <c r="G34" s="22">
+      <c r="G34" s="21">
         <v>65</v>
       </c>
-      <c r="H34" s="22">
+      <c r="H34" s="21">
         <f t="shared" si="0"/>
         <v>374</v>
       </c>
-      <c r="I34" s="22">
+      <c r="I34" s="21">
         <f t="shared" si="1"/>
         <v>74.8</v>
       </c>
-      <c r="J34" s="22" t="str">
+      <c r="J34" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="21">
         <v>82</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="21">
         <v>72</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="21">
         <v>98</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="21">
         <v>75</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="21">
         <v>65</v>
       </c>
-      <c r="H35" s="22">
+      <c r="H35" s="21">
         <f t="shared" si="0"/>
         <v>392</v>
       </c>
-      <c r="I35" s="22">
+      <c r="I35" s="21">
         <f t="shared" si="1"/>
         <v>78.400000000000006</v>
       </c>
-      <c r="J35" s="22" t="str">
+      <c r="J35" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="21">
         <v>92</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="21">
         <v>84</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="21">
         <v>32</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="21">
         <v>93</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="21">
         <v>94</v>
       </c>
-      <c r="H36" s="22">
+      <c r="H36" s="21">
         <f t="shared" si="0"/>
         <v>395</v>
       </c>
-      <c r="I36" s="22">
+      <c r="I36" s="21">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="J36" s="22" t="str">
+      <c r="J36" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="21">
         <v>97</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="21">
         <v>82</v>
       </c>
-      <c r="E37" s="22">
+      <c r="E37" s="21">
         <v>62</v>
       </c>
-      <c r="F37" s="22">
+      <c r="F37" s="21">
         <v>90</v>
       </c>
-      <c r="G37" s="22">
+      <c r="G37" s="21">
         <v>87</v>
       </c>
-      <c r="H37" s="22">
+      <c r="H37" s="21">
         <f t="shared" si="0"/>
         <v>418</v>
       </c>
-      <c r="I37" s="22">
+      <c r="I37" s="21">
         <f t="shared" si="1"/>
         <v>83.6</v>
       </c>
-      <c r="J37" s="22" t="str">
+      <c r="J37" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="21">
         <v>66</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="21">
         <v>86</v>
       </c>
-      <c r="E38" s="22">
+      <c r="E38" s="21">
         <v>61</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="21">
         <v>71</v>
       </c>
-      <c r="G38" s="22">
+      <c r="G38" s="21">
         <v>75</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="21">
         <f t="shared" si="0"/>
         <v>359</v>
       </c>
-      <c r="I38" s="22">
+      <c r="I38" s="21">
         <f t="shared" si="1"/>
         <v>71.8</v>
       </c>
-      <c r="J38" s="22" t="str">
+      <c r="J38" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="21">
         <v>65</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="21">
         <v>92</v>
       </c>
-      <c r="E39" s="22">
+      <c r="E39" s="21">
         <v>88</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="21">
         <v>63</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G39" s="21">
         <v>62</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="21">
         <f t="shared" si="0"/>
         <v>370</v>
       </c>
-      <c r="I39" s="22">
+      <c r="I39" s="21">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="J39" s="22" t="str">
+      <c r="J39" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="21">
         <v>70</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="21">
         <v>95</v>
       </c>
-      <c r="E40" s="22">
+      <c r="E40" s="21">
         <v>96</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="21">
         <v>85</v>
       </c>
-      <c r="G40" s="22">
+      <c r="G40" s="21">
         <v>63</v>
       </c>
-      <c r="H40" s="22">
+      <c r="H40" s="21">
         <f t="shared" si="0"/>
         <v>409</v>
       </c>
-      <c r="I40" s="22">
+      <c r="I40" s="21">
         <f t="shared" si="1"/>
         <v>81.8</v>
       </c>
-      <c r="J40" s="22" t="str">
+      <c r="J40" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="21">
         <v>68</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="21">
         <v>75</v>
       </c>
-      <c r="E41" s="22">
+      <c r="E41" s="21">
         <v>94</v>
       </c>
-      <c r="F41" s="22">
+      <c r="F41" s="21">
         <v>93</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="21">
         <v>75</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H41" s="21">
         <f t="shared" si="0"/>
         <v>405</v>
       </c>
-      <c r="I41" s="22">
+      <c r="I41" s="21">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="J41" s="22" t="str">
+      <c r="J41" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B42" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="21">
         <v>98</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="21">
         <v>64</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E42" s="21">
         <v>100</v>
       </c>
-      <c r="F42" s="22">
+      <c r="F42" s="21">
         <v>64</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="21">
         <v>72</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H42" s="21">
         <f t="shared" si="0"/>
         <v>398</v>
       </c>
-      <c r="I42" s="22">
+      <c r="I42" s="21">
         <f t="shared" si="1"/>
         <v>79.599999999999994</v>
       </c>
-      <c r="J42" s="22" t="str">
+      <c r="J42" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="23" t="s">
+      <c r="B43" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="21">
         <v>32</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="21">
         <v>80</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E43" s="21">
         <v>80</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F43" s="21">
         <v>77</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G43" s="21">
         <v>67</v>
       </c>
-      <c r="H43" s="22">
+      <c r="H43" s="21">
         <f t="shared" si="0"/>
         <v>336</v>
       </c>
-      <c r="I43" s="22">
+      <c r="I43" s="21">
         <f t="shared" si="1"/>
         <v>67.2</v>
       </c>
-      <c r="J43" s="22" t="str">
+      <c r="J43" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="B44" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="21">
         <v>85</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="21">
         <v>71</v>
       </c>
-      <c r="E44" s="22">
+      <c r="E44" s="21">
         <v>86</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="21">
         <v>65</v>
       </c>
-      <c r="G44" s="22">
+      <c r="G44" s="21">
         <v>83</v>
       </c>
-      <c r="H44" s="22">
+      <c r="H44" s="21">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
-      <c r="I44" s="22">
+      <c r="I44" s="21">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="J44" s="22" t="str">
+      <c r="J44" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="23" t="s">
+      <c r="B45" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="22">
+      <c r="C45" s="21">
         <v>87</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="21">
         <v>84</v>
       </c>
-      <c r="E45" s="22">
+      <c r="E45" s="21">
         <v>78</v>
       </c>
-      <c r="F45" s="22">
+      <c r="F45" s="21">
         <v>65</v>
       </c>
-      <c r="G45" s="22">
+      <c r="G45" s="21">
         <v>87</v>
       </c>
-      <c r="H45" s="22">
+      <c r="H45" s="21">
         <f t="shared" si="0"/>
         <v>401</v>
       </c>
-      <c r="I45" s="22">
+      <c r="I45" s="21">
         <f t="shared" si="1"/>
         <v>80.2</v>
       </c>
-      <c r="J45" s="22" t="str">
+      <c r="J45" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="21">
         <v>94</v>
       </c>
-      <c r="D46" s="22">
+      <c r="D46" s="21">
         <v>79</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="21">
         <v>73</v>
       </c>
-      <c r="F46" s="22">
+      <c r="F46" s="21">
         <v>62</v>
       </c>
-      <c r="G46" s="22">
+      <c r="G46" s="21">
         <v>88</v>
       </c>
-      <c r="H46" s="22">
+      <c r="H46" s="21">
         <f t="shared" si="0"/>
         <v>396</v>
       </c>
-      <c r="I46" s="22">
+      <c r="I46" s="21">
         <f t="shared" si="1"/>
         <v>79.2</v>
       </c>
-      <c r="J46" s="22" t="str">
+      <c r="J46" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="21">
         <v>77</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="21">
         <v>76</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="21">
         <v>72</v>
       </c>
-      <c r="F47" s="22">
+      <c r="F47" s="21">
         <v>77</v>
       </c>
-      <c r="G47" s="22">
+      <c r="G47" s="21">
         <v>80</v>
       </c>
-      <c r="H47" s="22">
+      <c r="H47" s="21">
         <f t="shared" si="0"/>
         <v>382</v>
       </c>
-      <c r="I47" s="22">
+      <c r="I47" s="21">
         <f t="shared" si="1"/>
         <v>76.400000000000006</v>
       </c>
-      <c r="J47" s="22" t="str">
+      <c r="J47" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="22">
+      <c r="C48" s="21">
         <v>85</v>
       </c>
-      <c r="D48" s="22">
+      <c r="D48" s="21">
         <v>98</v>
       </c>
-      <c r="E48" s="22">
+      <c r="E48" s="21">
         <v>82</v>
       </c>
-      <c r="F48" s="22">
+      <c r="F48" s="21">
         <v>99</v>
       </c>
-      <c r="G48" s="22">
+      <c r="G48" s="21">
         <v>82</v>
       </c>
-      <c r="H48" s="22">
+      <c r="H48" s="21">
         <f t="shared" si="0"/>
         <v>446</v>
       </c>
-      <c r="I48" s="22">
+      <c r="I48" s="21">
         <f t="shared" si="1"/>
         <v>89.2</v>
       </c>
-      <c r="J48" s="22" t="str">
+      <c r="J48" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="23" t="s">
+      <c r="B49" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="21">
         <v>65</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="21">
         <v>90</v>
       </c>
-      <c r="E49" s="22">
+      <c r="E49" s="21">
         <v>73</v>
       </c>
-      <c r="F49" s="22">
+      <c r="F49" s="21">
         <v>73</v>
       </c>
-      <c r="G49" s="22">
+      <c r="G49" s="21">
         <v>80</v>
       </c>
-      <c r="H49" s="22">
+      <c r="H49" s="21">
         <f t="shared" si="0"/>
         <v>381</v>
       </c>
-      <c r="I49" s="22">
+      <c r="I49" s="21">
         <f t="shared" si="1"/>
         <v>76.2</v>
       </c>
-      <c r="J49" s="22" t="str">
+      <c r="J49" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="22">
+      <c r="C50" s="21">
         <v>45</v>
       </c>
-      <c r="D50" s="22">
+      <c r="D50" s="21">
         <v>66</v>
       </c>
-      <c r="E50" s="22">
+      <c r="E50" s="21">
         <v>70</v>
       </c>
-      <c r="F50" s="22">
+      <c r="F50" s="21">
         <v>31</v>
       </c>
-      <c r="G50" s="22">
+      <c r="G50" s="21">
         <v>56</v>
       </c>
-      <c r="H50" s="22">
+      <c r="H50" s="21">
         <f t="shared" si="0"/>
         <v>268</v>
       </c>
-      <c r="I50" s="22">
+      <c r="I50" s="21">
         <f t="shared" si="1"/>
         <v>53.6</v>
       </c>
-      <c r="J50" s="22" t="str">
+      <c r="J50" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Fail</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C51" s="22">
+      <c r="C51" s="21">
         <v>61</v>
       </c>
-      <c r="D51" s="22">
+      <c r="D51" s="21">
         <v>93</v>
       </c>
-      <c r="E51" s="22">
+      <c r="E51" s="21">
         <v>80</v>
       </c>
-      <c r="F51" s="22">
+      <c r="F51" s="21">
         <v>60</v>
       </c>
-      <c r="G51" s="22">
+      <c r="G51" s="21">
         <v>76</v>
       </c>
-      <c r="H51" s="22">
+      <c r="H51" s="21">
         <f t="shared" si="0"/>
         <v>370</v>
       </c>
-      <c r="I51" s="22">
+      <c r="I51" s="21">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="J51" s="22" t="str">
+      <c r="J51" s="21" t="str">
         <f t="shared" si="2"/>
         <v>Pass</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="C2:G51">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
-      <formula>$O$1</formula>
+  <conditionalFormatting sqref="A2:J51">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$J2=$Q$3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J51">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$J2=$Q$3</formula>
+  <conditionalFormatting sqref="C2:G51">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>$O$1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10195,11 +11003,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF75E77F-8A53-495B-8423-338ED4416D93}">
+  <dimension ref="A1:T12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="41.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T1" s="12" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H12" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T1" r:id="rId1" xr:uid="{53E3E1CA-50B7-44EB-8C87-0AE065EA96D1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BBF5D9-8FB7-42E4-B0A4-B8AC86EC7EE1}">
   <dimension ref="A1:AJ51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10214,6 +11060,7 @@
     <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="57.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -11712,12 +12559,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4979C08-6F67-4EBD-8816-064FDFF2B18B}">
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11732,7 +12579,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -12910,7 +13757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5639990B-6750-4226-8125-85B5B2D017B4}">
   <dimension ref="A1:N24"/>
   <sheetViews>
@@ -13156,7 +14003,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2151C0B-73BA-4D05-A62D-E4D9FD47320B}">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -13213,7 +14060,7 @@
       <c r="C2" t="s">
         <v>664</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <v>42535</v>
       </c>
       <c r="E2">
@@ -13239,7 +14086,7 @@
       <c r="C3" t="s">
         <v>669</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>42748</v>
       </c>
       <c r="E3">
@@ -13265,7 +14112,7 @@
       <c r="C4" t="s">
         <v>673</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <v>42651</v>
       </c>
       <c r="E4">
@@ -13291,7 +14138,7 @@
       <c r="C5" t="s">
         <v>676</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <v>43222</v>
       </c>
       <c r="E5">
@@ -13317,7 +14164,7 @@
       <c r="C6" t="s">
         <v>679</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <v>42765</v>
       </c>
       <c r="E6">
@@ -13343,7 +14190,7 @@
       <c r="C7" t="s">
         <v>683</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <v>42101</v>
       </c>
       <c r="E7">
@@ -13369,7 +14216,7 @@
       <c r="C8" t="s">
         <v>686</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <v>41704</v>
       </c>
       <c r="E8">
@@ -13395,7 +14242,7 @@
       <c r="C9" t="s">
         <v>676</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <v>43244</v>
       </c>
       <c r="E9">
@@ -13421,7 +14268,7 @@
       <c r="C10" t="s">
         <v>692</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <v>41962</v>
       </c>
       <c r="E10">
@@ -13452,356 +14299,6 @@
       <c r="J17" t="str">
         <f>VLOOKUP(I17,A1:H10,2,0)</f>
         <v>Phonics Song with TWO Words - A For Apple - ABC Alphabet Songs with Sounds for Children</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C35B6DA-4005-4159-8F42-B0AFAD2CF07B}">
-  <dimension ref="A1:I21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>663</v>
-      </c>
-      <c r="C2" t="s">
-        <v>664</v>
-      </c>
-      <c r="D2" s="24">
-        <v>42535</v>
-      </c>
-      <c r="E2">
-        <v>12495185438</v>
-      </c>
-      <c r="F2" t="s">
-        <v>665</v>
-      </c>
-      <c r="G2" t="s">
-        <v>666</v>
-      </c>
-      <c r="H2" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>668</v>
-      </c>
-      <c r="C3" t="s">
-        <v>669</v>
-      </c>
-      <c r="D3" s="24">
-        <v>42748</v>
-      </c>
-      <c r="E3">
-        <v>8109237463</v>
-      </c>
-      <c r="F3" t="s">
-        <v>665</v>
-      </c>
-      <c r="G3" t="s">
-        <v>670</v>
-      </c>
-      <c r="H3" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C4" t="s">
-        <v>673</v>
-      </c>
-      <c r="D4" s="24">
-        <v>42651</v>
-      </c>
-      <c r="E4">
-        <v>6653263786</v>
-      </c>
-      <c r="F4" t="s">
-        <v>665</v>
-      </c>
-      <c r="G4" t="s">
-        <v>666</v>
-      </c>
-      <c r="H4" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>675</v>
-      </c>
-      <c r="C5" t="s">
-        <v>676</v>
-      </c>
-      <c r="D5" s="24">
-        <v>43222</v>
-      </c>
-      <c r="E5">
-        <v>6071073952</v>
-      </c>
-      <c r="F5" t="s">
-        <v>665</v>
-      </c>
-      <c r="G5" t="s">
-        <v>666</v>
-      </c>
-      <c r="H5" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>678</v>
-      </c>
-      <c r="C6" t="s">
-        <v>679</v>
-      </c>
-      <c r="D6" s="24">
-        <v>42765</v>
-      </c>
-      <c r="E6">
-        <v>5944830525</v>
-      </c>
-      <c r="F6" t="s">
-        <v>680</v>
-      </c>
-      <c r="G6" t="s">
-        <v>666</v>
-      </c>
-      <c r="H6" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>682</v>
-      </c>
-      <c r="C7" t="s">
-        <v>683</v>
-      </c>
-      <c r="D7" s="24">
-        <v>42101</v>
-      </c>
-      <c r="E7">
-        <v>5816307940</v>
-      </c>
-      <c r="F7" t="s">
-        <v>665</v>
-      </c>
-      <c r="G7" t="s">
-        <v>666</v>
-      </c>
-      <c r="H7" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>685</v>
-      </c>
-      <c r="C8" t="s">
-        <v>686</v>
-      </c>
-      <c r="D8" s="24">
-        <v>41704</v>
-      </c>
-      <c r="E8">
-        <v>5209038987</v>
-      </c>
-      <c r="F8" t="s">
-        <v>687</v>
-      </c>
-      <c r="G8" t="s">
-        <v>666</v>
-      </c>
-      <c r="H8" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>689</v>
-      </c>
-      <c r="C9" t="s">
-        <v>676</v>
-      </c>
-      <c r="D9" s="24">
-        <v>43244</v>
-      </c>
-      <c r="E9">
-        <v>5021165699</v>
-      </c>
-      <c r="F9" t="s">
-        <v>665</v>
-      </c>
-      <c r="G9" t="s">
-        <v>666</v>
-      </c>
-      <c r="H9" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>691</v>
-      </c>
-      <c r="C10" t="s">
-        <v>692</v>
-      </c>
-      <c r="D10" s="24">
-        <v>41962</v>
-      </c>
-      <c r="E10">
-        <v>4859631966</v>
-      </c>
-      <c r="F10" t="s">
-        <v>665</v>
-      </c>
-      <c r="G10" t="s">
-        <v>666</v>
-      </c>
-      <c r="H10" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G17" t="s">
-        <v>655</v>
-      </c>
-      <c r="H17" t="s">
-        <v>657</v>
-      </c>
-      <c r="I17" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18" t="str">
-        <f>VLOOKUP($G18,$A$1:$H$10,3,FALSE)</f>
-        <v>LuisFonsiVEVO</v>
-      </c>
-      <c r="I18">
-        <f>VLOOKUP($G18,$A$1:$H$10,5,FALSE)</f>
-        <v>8109237463</v>
-      </c>
-    </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19">
-        <v>5</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" ref="H19:H21" si="0">VLOOKUP($G19,$A$1:$H$10,3,FALSE)</f>
-        <v>Ed Sheeran</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ref="I19:I21" si="1">VLOOKUP($G19,$A$1:$H$10,5,FALSE)</f>
-        <v>5944830525</v>
-      </c>
-    </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G20">
-        <v>6</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>Wiz Khalifa</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>5816307940</v>
-      </c>
-    </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G21">
-        <v>9</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>MarkRonsonVEVO</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>4859631966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PQ sample datasets added
</commit_message>
<xml_diff>
--- a/excel-beginner-tutorial.xlsx
+++ b/excel-beginner-tutorial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub Projects\microsoft-excel-tutorial-beginner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2673B57F-3C4C-46E9-B9B1-EEBF6212F491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC68DF3-F383-4671-B6EE-E2B408687E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="7" activeTab="15" xr2:uid="{9FA7835E-DA76-4B93-946E-CCC2848369CA}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3225,7 +3225,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3277,7 +3277,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -5769,7 +5768,7 @@
   <dimension ref="A1:L108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9207,7 +9206,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B8"/>
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9550,7 +9549,7 @@
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14747,9 +14746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BBF5D9-8FB7-42E4-B0A4-B8AC86EC7EE1}">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15207,9 +15204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E2969B-5042-435B-96EE-9A63113DCFD9}">
   <dimension ref="A1:AH9097"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15277,7 +15272,7 @@
       <c r="N1" s="2" t="s">
         <v>969</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="4" t="s">
         <v>967</v>
       </c>
       <c r="V1" s="4"/>
@@ -15335,7 +15330,7 @@
       </c>
       <c r="O2" s="39">
         <f ca="1">TODAY()</f>
-        <v>45015</v>
+        <v>45016</v>
       </c>
       <c r="V2" s="4"/>
     </row>
@@ -15421,7 +15416,7 @@
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="3"/>
-        <v>22.21</v>
+        <v>22.22</v>
       </c>
       <c r="V4" s="4"/>
     </row>
@@ -15550,7 +15545,7 @@
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="3"/>
-        <v>17.760000000000002</v>
+        <v>17.77</v>
       </c>
       <c r="V7" s="4"/>
     </row>
@@ -15593,7 +15588,7 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="3"/>
-        <v>17.149999999999999</v>
+        <v>17.16</v>
       </c>
       <c r="V8" s="4"/>
     </row>
@@ -15722,7 +15717,7 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="3"/>
-        <v>20.62</v>
+        <v>20.63</v>
       </c>
       <c r="V11" s="4"/>
     </row>
@@ -15851,7 +15846,7 @@
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="3"/>
-        <v>17.059999999999999</v>
+        <v>17.07</v>
       </c>
       <c r="V14" s="4"/>
     </row>
@@ -15894,7 +15889,7 @@
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="3"/>
-        <v>15.31</v>
+        <v>15.32</v>
       </c>
       <c r="V15" s="4"/>
     </row>
@@ -15937,7 +15932,7 @@
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
-        <v>20.309999999999999</v>
+        <v>20.32</v>
       </c>
       <c r="V16" s="4"/>
     </row>
@@ -16064,7 +16059,7 @@
       </c>
       <c r="L19">
         <f t="shared" ca="1" si="3"/>
-        <v>17.68</v>
+        <v>17.690000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -16232,7 +16227,7 @@
       </c>
       <c r="L23">
         <f t="shared" ca="1" si="3"/>
-        <v>17.97</v>
+        <v>17.98</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -16274,7 +16269,7 @@
       </c>
       <c r="L24">
         <f t="shared" ca="1" si="3"/>
-        <v>19.91</v>
+        <v>19.920000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -16316,7 +16311,7 @@
       </c>
       <c r="L25">
         <f t="shared" ca="1" si="3"/>
-        <v>17.47</v>
+        <v>17.48</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -16358,7 +16353,7 @@
       </c>
       <c r="L26">
         <f t="shared" ca="1" si="3"/>
-        <v>15.37</v>
+        <v>15.38</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -16652,7 +16647,7 @@
       </c>
       <c r="L33">
         <f t="shared" ca="1" si="3"/>
-        <v>18.12</v>
+        <v>18.13</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -16694,7 +16689,7 @@
       </c>
       <c r="L34">
         <f t="shared" ca="1" si="3"/>
-        <v>15.97</v>
+        <v>15.98</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -16736,7 +16731,7 @@
       </c>
       <c r="L35">
         <f t="shared" ca="1" si="3"/>
-        <v>18.79</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -16778,7 +16773,7 @@
       </c>
       <c r="L36">
         <f t="shared" ca="1" si="3"/>
-        <v>16.59</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -16988,7 +16983,7 @@
       </c>
       <c r="L41">
         <f t="shared" ca="1" si="3"/>
-        <v>17.13</v>
+        <v>17.14</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -17030,7 +17025,7 @@
       </c>
       <c r="L42">
         <f t="shared" ca="1" si="3"/>
-        <v>16.98</v>
+        <v>16.989999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -17072,7 +17067,7 @@
       </c>
       <c r="L43">
         <f t="shared" ca="1" si="3"/>
-        <v>19.45</v>
+        <v>19.46</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -17660,7 +17655,7 @@
       </c>
       <c r="L57">
         <f t="shared" ca="1" si="3"/>
-        <v>15.35</v>
+        <v>15.36</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -17744,7 +17739,7 @@
       </c>
       <c r="L59">
         <f t="shared" ca="1" si="3"/>
-        <v>19.07</v>
+        <v>19.079999999999998</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -17786,7 +17781,7 @@
       </c>
       <c r="L60">
         <f t="shared" ca="1" si="3"/>
-        <v>18.66</v>
+        <v>18.670000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -18038,7 +18033,7 @@
       </c>
       <c r="L66">
         <f t="shared" ca="1" si="3"/>
-        <v>15.18</v>
+        <v>15.19</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -18080,7 +18075,7 @@
       </c>
       <c r="L67">
         <f t="shared" ref="L67:L108" ca="1" si="7">ROUND(YEARFRAC(G67,$O$2),2)</f>
-        <v>15.1</v>
+        <v>15.11</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -18206,7 +18201,7 @@
       </c>
       <c r="L70">
         <f t="shared" ca="1" si="7"/>
-        <v>18.05</v>
+        <v>18.059999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -18290,7 +18285,7 @@
       </c>
       <c r="L72">
         <f t="shared" ca="1" si="7"/>
-        <v>17.18</v>
+        <v>17.190000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -18332,7 +18327,7 @@
       </c>
       <c r="L73">
         <f t="shared" ca="1" si="7"/>
-        <v>16.100000000000001</v>
+        <v>16.11</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -18710,7 +18705,7 @@
       </c>
       <c r="L82">
         <f t="shared" ca="1" si="7"/>
-        <v>17.18</v>
+        <v>17.190000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -18752,7 +18747,7 @@
       </c>
       <c r="L83">
         <f t="shared" ca="1" si="7"/>
-        <v>17.100000000000001</v>
+        <v>17.11</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -19046,7 +19041,7 @@
       </c>
       <c r="L90">
         <f t="shared" ca="1" si="7"/>
-        <v>17.79</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -19382,7 +19377,7 @@
       </c>
       <c r="L98">
         <f t="shared" ca="1" si="7"/>
-        <v>16.93</v>
+        <v>16.940000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -19424,7 +19419,7 @@
       </c>
       <c r="L99">
         <f t="shared" ca="1" si="7"/>
-        <v>16.850000000000001</v>
+        <v>16.86</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -19508,7 +19503,7 @@
       </c>
       <c r="L101">
         <f t="shared" ca="1" si="7"/>
-        <v>15.21</v>
+        <v>15.22</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -19676,7 +19671,7 @@
       </c>
       <c r="L105">
         <f t="shared" ca="1" si="7"/>
-        <v>20.81</v>
+        <v>20.82</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -19718,7 +19713,7 @@
       </c>
       <c r="L106">
         <f t="shared" ca="1" si="7"/>
-        <v>20.81</v>
+        <v>20.82</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -19760,7 +19755,7 @@
       </c>
       <c r="L107">
         <f t="shared" ca="1" si="7"/>
-        <v>20.81</v>
+        <v>20.82</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -19802,7 +19797,7 @@
       </c>
       <c r="L108">
         <f t="shared" ca="1" si="7"/>
-        <v>20.81</v>
+        <v>20.82</v>
       </c>
     </row>
     <row r="9097" spans="10:10" x14ac:dyDescent="0.25">
@@ -19847,7 +19842,7 @@
       </c>
       <c r="B2" s="33">
         <f ca="1">TODAY()</f>
-        <v>45015</v>
+        <v>45016</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>335</v>
@@ -19859,7 +19854,7 @@
       </c>
       <c r="B3" s="35">
         <f ca="1">NOW()</f>
-        <v>45015.88874490741</v>
+        <v>45016.260167824075</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>337</v>
@@ -19895,7 +19890,7 @@
       </c>
       <c r="B6" s="34">
         <f ca="1">DAY(B2)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>343</v>
@@ -19907,7 +19902,7 @@
       </c>
       <c r="B7" s="34">
         <f ca="1">HOUR(B3)</f>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>345</v>
@@ -19919,7 +19914,7 @@
       </c>
       <c r="B8" s="34">
         <f ca="1">MINUTE(B3)</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C8" s="34" t="s">
         <v>347</v>
@@ -19931,7 +19926,7 @@
       </c>
       <c r="B9" s="34">
         <f ca="1">SECOND(B3)</f>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>349</v>
@@ -19997,7 +19992,7 @@
       </c>
       <c r="B14" s="33">
         <f ca="1">WORKDAY(B2,B6)</f>
-        <v>45057</v>
+        <v>45061</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>361</v>
@@ -20009,7 +20004,7 @@
       </c>
       <c r="B15" s="33">
         <f ca="1">WORKDAY.INTL(B2,B6,1)</f>
-        <v>45057</v>
+        <v>45061</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>363</v>
@@ -20021,7 +20016,7 @@
       </c>
       <c r="B16" s="34">
         <f ca="1">NETWORKDAYS(B2,B10)</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>365</v>
@@ -20033,7 +20028,7 @@
       </c>
       <c r="B17" s="34">
         <f ca="1">NETWORKDAYS.INTL(B2,B10,1)</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>367</v>
@@ -20045,7 +20040,7 @@
       </c>
       <c r="B18" s="37">
         <f ca="1">DATE(B4,B5,B6)</f>
-        <v>45015</v>
+        <v>45016</v>
       </c>
       <c r="C18" s="34" t="s">
         <v>369</v>
@@ -20057,7 +20052,7 @@
       </c>
       <c r="B19" s="38">
         <f ca="1">TIME(B7,B8,B9)</f>
-        <v>0.88874999999999993</v>
+        <v>0.26016203703703705</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>371</v>
@@ -20069,7 +20064,7 @@
       </c>
       <c r="B20" s="34">
         <f ca="1">WEEKDAY(B2,1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>373</v>
@@ -20081,7 +20076,7 @@
       </c>
       <c r="B21" s="34">
         <f ca="1">WEEKDAY(B2,1)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>373</v>
@@ -20093,7 +20088,7 @@
       </c>
       <c r="B22" s="34">
         <f ca="1">_xlfn.DAYS(B10,B2)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>376</v>
@@ -20117,7 +20112,7 @@
       </c>
       <c r="B24" s="34">
         <f ca="1">DATEDIF(B2,B11,"D")</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="34" t="s">
         <v>380</v>

</xml_diff>